<commit_message>
Corrigindo algumas planilhas e adicionando o dicionario de Graham.
</commit_message>
<xml_diff>
--- a/Data_frame/balancos_definitivos/AALR3.xlsx
+++ b/Data_frame/balancos_definitivos/AALR3.xlsx
@@ -333,7 +333,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,13 +343,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -396,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -407,22 +401,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -736,42 +721,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="54.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -5944,7 +5929,7 @@
         <v>1089045.04</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="3" t="s">
         <v>72</v>
       </c>
@@ -6054,7 +6039,7 @@
         <v>612412.032</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="3" t="s">
         <v>73</v>
       </c>
@@ -6164,7 +6149,7 @@
         <v>1060798.976</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="3" t="s">
         <v>74</v>
       </c>
@@ -6274,7 +6259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="3" t="s">
         <v>75</v>
       </c>
@@ -6384,7 +6369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="3" t="s">
         <v>76</v>
       </c>
@@ -6494,7 +6479,7 @@
         <v>-584166.016</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="3" t="s">
         <v>77</v>
       </c>
@@ -6604,7 +6589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="3" t="s">
         <v>78</v>
       </c>
@@ -6714,7 +6699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="3" t="s">
         <v>79</v>
       </c>
@@ -6824,7 +6809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="3" t="s">
         <v>68</v>
       </c>
@@ -6934,91 +6919,91 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B57" s="6"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
-      <c r="R57" s="7"/>
-      <c r="S57" s="7"/>
-      <c r="T57" s="7"/>
-      <c r="U57" s="7"/>
-      <c r="V57" s="7"/>
-      <c r="W57" s="7"/>
-      <c r="X57" s="7"/>
-      <c r="Y57" s="7"/>
-      <c r="Z57" s="7"/>
-      <c r="AA57" s="7"/>
-      <c r="AB57" s="7"/>
-      <c r="AC57" s="7"/>
-      <c r="AD57" s="7"/>
-      <c r="AE57" s="7"/>
-      <c r="AF57" s="7"/>
-      <c r="AG57" s="7"/>
-      <c r="AH57" s="7"/>
-      <c r="AI57" s="7"/>
-      <c r="AJ57" s="7"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4"/>
+      <c r="AB57" s="4"/>
+      <c r="AC57" s="4"/>
+      <c r="AD57" s="4"/>
+      <c r="AE57" s="4"/>
+      <c r="AF57" s="4"/>
+      <c r="AG57" s="4"/>
+      <c r="AH57" s="4"/>
+      <c r="AI57" s="4"/>
+      <c r="AJ57" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B58" s="6"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="7"/>
-      <c r="P58" s="7"/>
-      <c r="Q58" s="7"/>
-      <c r="R58" s="7"/>
-      <c r="S58" s="7"/>
-      <c r="T58" s="7"/>
-      <c r="U58" s="7"/>
-      <c r="V58" s="7"/>
-      <c r="W58" s="7"/>
-      <c r="X58" s="7"/>
-      <c r="Y58" s="7"/>
-      <c r="Z58" s="7"/>
-      <c r="AA58" s="7"/>
-      <c r="AB58" s="7"/>
-      <c r="AC58" s="7"/>
-      <c r="AD58" s="7"/>
-      <c r="AE58" s="7"/>
-      <c r="AF58" s="7"/>
-      <c r="AG58" s="7"/>
-      <c r="AH58" s="7"/>
-      <c r="AI58" s="7"/>
-      <c r="AJ58" s="7"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="4"/>
+      <c r="AA58" s="4"/>
+      <c r="AB58" s="4"/>
+      <c r="AC58" s="4"/>
+      <c r="AD58" s="4"/>
+      <c r="AE58" s="4"/>
+      <c r="AF58" s="4"/>
+      <c r="AG58" s="4"/>
+      <c r="AH58" s="4"/>
+      <c r="AI58" s="4"/>
+      <c r="AJ58" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B59" s="6"/>
+      <c r="B59" s="4"/>
       <c r="C59" s="4">
         <v>195726</v>
       </c>
@@ -7122,11 +7107,11 @@
         <v>317736</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B60" s="6"/>
+      <c r="B60" s="4"/>
       <c r="C60" s="4">
         <v>-121658</v>
       </c>
@@ -7230,11 +7215,11 @@
         <v>-219575.008</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="6"/>
+      <c r="B61" s="4"/>
       <c r="C61" s="4">
         <v>74068</v>
       </c>
@@ -7338,11 +7323,11 @@
         <v>98161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="6"/>
+      <c r="B62" s="4"/>
       <c r="C62" s="4">
         <v>0</v>
       </c>
@@ -7446,11 +7431,11 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="6"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="4">
         <v>-47437</v>
       </c>
@@ -7554,11 +7539,11 @@
         <v>-55208</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B64" s="6"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="4">
         <v>0</v>
       </c>
@@ -7662,11 +7647,11 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B65" s="6"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="4">
         <v>0</v>
       </c>
@@ -7770,11 +7755,11 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B66" s="6"/>
+      <c r="B66" s="4"/>
       <c r="C66" s="4">
         <v>-5099</v>
       </c>
@@ -7878,11 +7863,11 @@
         <v>962</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B67" s="6"/>
+      <c r="B67" s="4"/>
       <c r="C67" s="4">
         <v>1129</v>
       </c>
@@ -7986,11 +7971,11 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="6"/>
+      <c r="B68" s="4"/>
       <c r="C68" s="4">
         <v>-6948</v>
       </c>
@@ -8094,11 +8079,11 @@
         <v>-40276</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B69" s="6"/>
+      <c r="B69" s="4"/>
       <c r="C69" s="4">
         <v>0</v>
       </c>
@@ -8202,11 +8187,11 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B70" s="6"/>
+      <c r="B70" s="4"/>
       <c r="C70" s="4">
         <v>0</v>
       </c>
@@ -8310,131 +8295,131 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B71" s="6"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
-      <c r="N71" s="7"/>
-      <c r="O71" s="7"/>
-      <c r="P71" s="7"/>
-      <c r="Q71" s="7"/>
-      <c r="R71" s="7"/>
-      <c r="S71" s="7"/>
-      <c r="T71" s="7"/>
-      <c r="U71" s="7"/>
-      <c r="V71" s="7"/>
-      <c r="W71" s="7"/>
-      <c r="X71" s="7"/>
-      <c r="Y71" s="7"/>
-      <c r="Z71" s="7"/>
-      <c r="AA71" s="7"/>
-      <c r="AB71" s="7"/>
-      <c r="AC71" s="7"/>
-      <c r="AD71" s="7"/>
-      <c r="AE71" s="7"/>
-      <c r="AF71" s="7"/>
-      <c r="AG71" s="7"/>
-      <c r="AH71" s="7"/>
-      <c r="AI71" s="7"/>
-      <c r="AJ71" s="7"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4"/>
+      <c r="Q71" s="4"/>
+      <c r="R71" s="4"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4"/>
+      <c r="U71" s="4"/>
+      <c r="V71" s="4"/>
+      <c r="W71" s="4"/>
+      <c r="X71" s="4"/>
+      <c r="Y71" s="4"/>
+      <c r="Z71" s="4"/>
+      <c r="AA71" s="4"/>
+      <c r="AB71" s="4"/>
+      <c r="AC71" s="4"/>
+      <c r="AD71" s="4"/>
+      <c r="AE71" s="4"/>
+      <c r="AF71" s="4"/>
+      <c r="AG71" s="4"/>
+      <c r="AH71" s="4"/>
+      <c r="AI71" s="4"/>
+      <c r="AJ71" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B72" s="6"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="I72" s="7"/>
-      <c r="J72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
-      <c r="P72" s="7"/>
-      <c r="Q72" s="7"/>
-      <c r="R72" s="7"/>
-      <c r="S72" s="7"/>
-      <c r="T72" s="7"/>
-      <c r="U72" s="7"/>
-      <c r="V72" s="7"/>
-      <c r="W72" s="7"/>
-      <c r="X72" s="7"/>
-      <c r="Y72" s="7"/>
-      <c r="Z72" s="7"/>
-      <c r="AA72" s="7"/>
-      <c r="AB72" s="7"/>
-      <c r="AC72" s="7"/>
-      <c r="AD72" s="7"/>
-      <c r="AE72" s="7"/>
-      <c r="AF72" s="7"/>
-      <c r="AG72" s="7"/>
-      <c r="AH72" s="7"/>
-      <c r="AI72" s="7"/>
-      <c r="AJ72" s="7"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="4"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="4"/>
+      <c r="U72" s="4"/>
+      <c r="V72" s="4"/>
+      <c r="W72" s="4"/>
+      <c r="X72" s="4"/>
+      <c r="Y72" s="4"/>
+      <c r="Z72" s="4"/>
+      <c r="AA72" s="4"/>
+      <c r="AB72" s="4"/>
+      <c r="AC72" s="4"/>
+      <c r="AD72" s="4"/>
+      <c r="AE72" s="4"/>
+      <c r="AF72" s="4"/>
+      <c r="AG72" s="4"/>
+      <c r="AH72" s="4"/>
+      <c r="AI72" s="4"/>
+      <c r="AJ72" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="7"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7"/>
-      <c r="O73" s="7"/>
-      <c r="P73" s="7"/>
-      <c r="Q73" s="7"/>
-      <c r="R73" s="7"/>
-      <c r="S73" s="7"/>
-      <c r="T73" s="7"/>
-      <c r="U73" s="7"/>
-      <c r="V73" s="7"/>
-      <c r="W73" s="7"/>
-      <c r="X73" s="7"/>
-      <c r="Y73" s="7"/>
-      <c r="Z73" s="7"/>
-      <c r="AA73" s="7"/>
-      <c r="AB73" s="7"/>
-      <c r="AC73" s="7"/>
-      <c r="AD73" s="7"/>
-      <c r="AE73" s="7"/>
-      <c r="AF73" s="7"/>
-      <c r="AG73" s="7"/>
-      <c r="AH73" s="7"/>
-      <c r="AI73" s="7"/>
-      <c r="AJ73" s="7"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="4"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4"/>
+      <c r="U73" s="4"/>
+      <c r="V73" s="4"/>
+      <c r="W73" s="4"/>
+      <c r="X73" s="4"/>
+      <c r="Y73" s="4"/>
+      <c r="Z73" s="4"/>
+      <c r="AA73" s="4"/>
+      <c r="AB73" s="4"/>
+      <c r="AC73" s="4"/>
+      <c r="AD73" s="4"/>
+      <c r="AE73" s="4"/>
+      <c r="AF73" s="4"/>
+      <c r="AG73" s="4"/>
+      <c r="AH73" s="4"/>
+      <c r="AI73" s="4"/>
+      <c r="AJ73" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="6"/>
+      <c r="B74" s="4"/>
       <c r="C74" s="4">
         <v>15713</v>
       </c>
@@ -8538,11 +8523,11 @@
         <v>3639</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B75" s="6"/>
+      <c r="B75" s="4"/>
       <c r="C75" s="4">
         <v>0</v>
       </c>
@@ -8646,11 +8631,11 @@
         <v>-481</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B76" s="6"/>
+      <c r="B76" s="4"/>
       <c r="C76" s="4">
         <v>0</v>
       </c>
@@ -8754,91 +8739,91 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B77" s="6"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
-      <c r="I77" s="7"/>
-      <c r="J77" s="7"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="7"/>
-      <c r="M77" s="7"/>
-      <c r="N77" s="7"/>
-      <c r="O77" s="7"/>
-      <c r="P77" s="7"/>
-      <c r="Q77" s="7"/>
-      <c r="R77" s="7"/>
-      <c r="S77" s="7"/>
-      <c r="T77" s="7"/>
-      <c r="U77" s="7"/>
-      <c r="V77" s="7"/>
-      <c r="W77" s="7"/>
-      <c r="X77" s="7"/>
-      <c r="Y77" s="7"/>
-      <c r="Z77" s="7"/>
-      <c r="AA77" s="7"/>
-      <c r="AB77" s="7"/>
-      <c r="AC77" s="7"/>
-      <c r="AD77" s="7"/>
-      <c r="AE77" s="7"/>
-      <c r="AF77" s="7"/>
-      <c r="AG77" s="7"/>
-      <c r="AH77" s="7"/>
-      <c r="AI77" s="7"/>
-      <c r="AJ77" s="7"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="4"/>
+      <c r="U77" s="4"/>
+      <c r="V77" s="4"/>
+      <c r="W77" s="4"/>
+      <c r="X77" s="4"/>
+      <c r="Y77" s="4"/>
+      <c r="Z77" s="4"/>
+      <c r="AA77" s="4"/>
+      <c r="AB77" s="4"/>
+      <c r="AC77" s="4"/>
+      <c r="AD77" s="4"/>
+      <c r="AE77" s="4"/>
+      <c r="AF77" s="4"/>
+      <c r="AG77" s="4"/>
+      <c r="AH77" s="4"/>
+      <c r="AI77" s="4"/>
+      <c r="AJ77" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B78" s="6"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="7"/>
-      <c r="J78" s="7"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="7"/>
-      <c r="M78" s="7"/>
-      <c r="N78" s="7"/>
-      <c r="O78" s="7"/>
-      <c r="P78" s="7"/>
-      <c r="Q78" s="7"/>
-      <c r="R78" s="7"/>
-      <c r="S78" s="7"/>
-      <c r="T78" s="7"/>
-      <c r="U78" s="7"/>
-      <c r="V78" s="7"/>
-      <c r="W78" s="7"/>
-      <c r="X78" s="7"/>
-      <c r="Y78" s="7"/>
-      <c r="Z78" s="7"/>
-      <c r="AA78" s="7"/>
-      <c r="AB78" s="7"/>
-      <c r="AC78" s="7"/>
-      <c r="AD78" s="7"/>
-      <c r="AE78" s="7"/>
-      <c r="AF78" s="7"/>
-      <c r="AG78" s="7"/>
-      <c r="AH78" s="7"/>
-      <c r="AI78" s="7"/>
-      <c r="AJ78" s="7"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="4"/>
+      <c r="S78" s="4"/>
+      <c r="T78" s="4"/>
+      <c r="U78" s="4"/>
+      <c r="V78" s="4"/>
+      <c r="W78" s="4"/>
+      <c r="X78" s="4"/>
+      <c r="Y78" s="4"/>
+      <c r="Z78" s="4"/>
+      <c r="AA78" s="4"/>
+      <c r="AB78" s="4"/>
+      <c r="AC78" s="4"/>
+      <c r="AD78" s="4"/>
+      <c r="AE78" s="4"/>
+      <c r="AF78" s="4"/>
+      <c r="AG78" s="4"/>
+      <c r="AH78" s="4"/>
+      <c r="AI78" s="4"/>
+      <c r="AJ78" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B79" s="6"/>
+      <c r="B79" s="4"/>
       <c r="C79" s="4">
         <v>-2193</v>
       </c>
@@ -8942,11 +8927,11 @@
         <v>-2725</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B80" s="6"/>
+      <c r="B80" s="4"/>
       <c r="C80" s="4">
         <v>7532</v>
       </c>

</xml_diff>